<commit_message>
Grundsätzlich alles fertig. Bugs sollten ebenso behoben sein. - Belegungen können erzeugt werden. - Fächer können den einzelnen Lehrern zugeteilt werden.
</commit_message>
<xml_diff>
--- a/data/Klasse/5BHELS.xlsx
+++ b/data/Klasse/5BHELS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Stundenplan für 5BHELS</t>
   </si>
@@ -38,6 +38,16 @@
     <t>8:40</t>
   </si>
   <si>
+    <t>Hardwareentwicklung
+GERE
+W11x</t>
+  </si>
+  <si>
+    <t>Englisch
+RAKL
+W118</t>
+  </si>
+  <si>
     <t>9:30</t>
   </si>
   <si>
@@ -47,25 +57,15 @@
     <t>9:40</t>
   </si>
   <si>
+    <t>10:30</t>
+  </si>
+  <si>
     <t>Mathematik
-FIAL
-W118</t>
-  </si>
-  <si>
-    <t>10:30</t>
-  </si>
-  <si>
-    <t>Deutsch
 WÜBE
 W118</t>
   </si>
   <si>
     <t>11:20</t>
-  </si>
-  <si>
-    <t>Softwareentwicklung
-FIAL
-W118</t>
   </si>
   <si>
     <t>12:10</t>
@@ -141,8 +141,8 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="6.2578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="19.45703125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.13671875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.7265625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.48828125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="11.36328125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="7.16796875" customWidth="true" bestFit="true"/>
   </cols>
@@ -184,38 +184,40 @@
         <v>7</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" ht="45.0" customHeight="true">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -223,23 +225,21 @@
     </row>
     <row r="7" ht="45.0" customHeight="true">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" ht="45.0" customHeight="true">
       <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -250,19 +250,19 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" ht="45.0" customHeight="true">
@@ -300,19 +300,19 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" ht="45.0" customHeight="true">

</xml_diff>